<commit_message>
Added feature to ignore references in specified scripts
</commit_message>
<xml_diff>
--- a/TestWebApplication/JSBuilderConfig.xlsx
+++ b/TestWebApplication/JSBuilderConfig.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Build Includes</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Target HTML File</t>
   </si>
   <si>
-    <t>Source Folders</t>
-  </si>
-  <si>
     <t>Ignore References In:</t>
   </si>
   <si>
@@ -45,37 +42,25 @@
     <t>Tests.html</t>
   </si>
   <si>
-    <t>Scripts,Tests</t>
-  </si>
-  <si>
-    <t>jquery.signalR.js</t>
-  </si>
-  <si>
-    <t>Scripts</t>
-  </si>
-  <si>
-    <t>WebProject</t>
-  </si>
-  <si>
     <t>Tests\alltests.js</t>
   </si>
   <si>
     <t>Scripts\app.js</t>
   </si>
   <si>
-    <t>App.html</t>
-  </si>
-  <si>
     <t>TestWebApplication</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>Templates\Tests.template</t>
   </si>
   <si>
-    <t>Templates\App.template</t>
+    <t>Templates\Index.template</t>
+  </si>
+  <si>
+    <t>Index.html</t>
+  </si>
+  <si>
+    <t>libWithBadRef.js</t>
   </si>
 </sst>
 </file>
@@ -131,15 +116,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G3" totalsRowShown="0">
-  <autoFilter ref="A1:G3"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F3" totalsRowShown="0">
+  <autoFilter ref="A1:F3"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Build Includes"/>
     <tableColumn id="2" name="Web Application Root Folder"/>
     <tableColumn id="3" name="Root Script"/>
     <tableColumn id="4" name="Source Template Path"/>
     <tableColumn id="5" name="Target HTML File"/>
-    <tableColumn id="6" name="Source Folders"/>
     <tableColumn id="7" name="Ignore References In:"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -433,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,11 +430,10 @@
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,54 +452,45 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>